<commit_message>
Further tweaks to experiment following @taylor13
</commit_message>
<xml_diff>
--- a/src/160713_CMIP6_expt_list.xlsx
+++ b/src/160713_CMIP6_expt_list.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1074">
   <si>
     <t>segments of experiment_id</t>
   </si>
@@ -3690,6 +3690,9 @@
   </si>
   <si>
     <t>Future SSP3-7.0 with reduced ozone precursor emissions (from ssp370-lowNTCF), prescribed SSTs</t>
+  </si>
+  <si>
+    <t>dcppA-assim</t>
   </si>
 </sst>
 </file>
@@ -5222,15 +5225,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5242,6 +5236,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1013">
@@ -6600,8 +6603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6633,55 +6636,55 @@
       <c r="A1" s="64" t="s">
         <v>624</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="79" t="s">
         <v>1013</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
     </row>
     <row r="2" spans="1:24" ht="132" customHeight="1">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="84" t="s">
         <v>861</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>871</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:24" s="6" customFormat="1" ht="160" customHeight="1">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85" t="s">
         <v>872</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
       <c r="Q3" s="41"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -6693,81 +6696,81 @@
       <c r="A4" s="63" t="s">
         <v>862</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="83" t="s">
         <v>625</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
     </row>
     <row r="5" spans="1:24" ht="50" customHeight="1">
       <c r="A5" s="63" t="s">
         <v>863</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="83" t="s">
         <v>728</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
     </row>
     <row r="6" spans="1:24" ht="35" customHeight="1">
       <c r="A6" s="63" t="s">
         <v>864</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="83" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
     </row>
     <row r="7" spans="1:24" ht="47" customHeight="1">
       <c r="A7" s="63" t="s">
         <v>857</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="83" t="s">
         <v>856</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
     </row>
     <row r="8" spans="1:24" ht="42" customHeight="1">
       <c r="A8" s="63" t="s">
         <v>727</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="83" t="s">
         <v>627</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
     </row>
     <row r="9" spans="1:24" ht="33" customHeight="1">
       <c r="A9" s="39"/>
@@ -6785,25 +6788,25 @@
       <c r="A10" s="35" t="s">
         <v>628</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="79" t="s">
         <v>1013</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
     </row>
     <row r="11" spans="1:24" ht="36" customHeight="1">
       <c r="C11" s="48" t="s">
@@ -6811,19 +6814,19 @@
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="48"/>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="81" t="s">
         <v>854</v>
       </c>
-      <c r="G11" s="84"/>
-      <c r="K11" s="83" t="s">
+      <c r="G11" s="81"/>
+      <c r="K11" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="O11" s="84" t="s">
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="O11" s="81" t="s">
         <v>873</v>
       </c>
-      <c r="P11" s="84"/>
+      <c r="P11" s="81"/>
       <c r="R11" s="67" t="s">
         <v>725</v>
       </c>
@@ -13727,7 +13730,7 @@
         <v>1018</v>
       </c>
       <c r="T108" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U108" s="36" t="str">
         <f t="shared" ref="U108:U140" si="24">IF(T108="", "", "none")</f>
@@ -13792,7 +13795,7 @@
         <v>1018</v>
       </c>
       <c r="T109" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U109" s="36" t="str">
         <f t="shared" si="24"/>
@@ -13976,7 +13979,7 @@
       </c>
       <c r="S112" s="10"/>
       <c r="T112" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U112" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14034,7 +14037,7 @@
       </c>
       <c r="S113" s="10"/>
       <c r="T113" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U113" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14106,7 +14109,7 @@
         <v>1018</v>
       </c>
       <c r="T114" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U114" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14179,7 +14182,7 @@
         <v>1018</v>
       </c>
       <c r="T115" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U115" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14250,7 +14253,7 @@
         <v>1018</v>
       </c>
       <c r="T116" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U116" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14309,7 +14312,7 @@
       </c>
       <c r="S117" s="10"/>
       <c r="T117" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U117" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14367,7 +14370,7 @@
       </c>
       <c r="S118" s="10"/>
       <c r="T118" s="73" t="s">
-        <v>1014</v>
+        <v>1073</v>
       </c>
       <c r="U118" s="36" t="str">
         <f t="shared" si="24"/>
@@ -25160,6 +25163,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B10:R10"/>
     <mergeCell ref="K11:M11"/>
@@ -25168,11 +25176,6 @@
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Further tweaks to experiment following #1
</commit_message>
<xml_diff>
--- a/src/160713_CMIP6_expt_list.xlsx
+++ b/src/160713_CMIP6_expt_list.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1073">
   <si>
     <t>segments of experiment_id</t>
   </si>
@@ -3489,9 +3489,6 @@
   </si>
   <si>
     <t>WARNING:  Columns D through I may not be reliable as they have not been confirmed by MIP leaders.</t>
-  </si>
-  <si>
-    <t>(dcppA-assim)</t>
   </si>
   <si>
     <t>number of char.</t>
@@ -3978,8 +3975,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1013">
+  <cellStyleXfs count="1015">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5225,6 +5224,15 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5237,17 +5245,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1013">
+  <cellStyles count="1015">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5754,6 +5753,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1014" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6260,6 +6260,7 @@
     <cellStyle name="Hyperlink" xfId="1007" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1009" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1013" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6603,8 +6604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="O190" workbookViewId="0">
+      <selection activeCell="T140" sqref="T140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6636,55 +6637,55 @@
       <c r="A1" s="64" t="s">
         <v>624</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="82" t="s">
         <v>1013</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
     </row>
     <row r="2" spans="1:24" ht="132" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="79" t="s">
         <v>861</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="85" t="s">
         <v>871</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="3" spans="1:24" s="6" customFormat="1" ht="160" customHeight="1">
-      <c r="A3" s="84"/>
-      <c r="B3" s="85" t="s">
+      <c r="A3" s="79"/>
+      <c r="B3" s="80" t="s">
         <v>872</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
       <c r="Q3" s="41"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -6696,81 +6697,81 @@
       <c r="A4" s="63" t="s">
         <v>862</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="81" t="s">
         <v>625</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:24" ht="50" customHeight="1">
       <c r="A5" s="63" t="s">
         <v>863</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="81" t="s">
         <v>728</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
     </row>
     <row r="6" spans="1:24" ht="35" customHeight="1">
       <c r="A6" s="63" t="s">
         <v>864</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="81" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
     </row>
     <row r="7" spans="1:24" ht="47" customHeight="1">
       <c r="A7" s="63" t="s">
         <v>857</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="81" t="s">
         <v>856</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
     </row>
     <row r="8" spans="1:24" ht="42" customHeight="1">
       <c r="A8" s="63" t="s">
         <v>727</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="81" t="s">
         <v>627</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
     </row>
     <row r="9" spans="1:24" ht="33" customHeight="1">
       <c r="A9" s="39"/>
@@ -6788,25 +6789,25 @@
       <c r="A10" s="35" t="s">
         <v>628</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="82" t="s">
         <v>1013</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
     </row>
     <row r="11" spans="1:24" ht="36" customHeight="1">
       <c r="C11" s="48" t="s">
@@ -6814,19 +6815,19 @@
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="48"/>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="84" t="s">
         <v>854</v>
       </c>
-      <c r="G11" s="81"/>
-      <c r="K11" s="80" t="s">
+      <c r="G11" s="84"/>
+      <c r="K11" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="O11" s="81" t="s">
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="O11" s="84" t="s">
         <v>873</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="84"/>
       <c r="R11" s="67" t="s">
         <v>725</v>
       </c>
@@ -6903,7 +6904,7 @@
         <v>626</v>
       </c>
       <c r="X12" s="61" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="30">
@@ -8069,7 +8070,7 @@
     </row>
     <row r="29" spans="1:24" ht="30">
       <c r="A29" s="11" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>48</v>
@@ -8262,7 +8263,7 @@
         <v>ssp370SST-ssp126Lu</v>
       </c>
       <c r="R31" s="19" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="S31" s="10" t="str">
         <f t="shared" si="3"/>
@@ -8385,7 +8386,7 @@
         <v>piClim-NTCF</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="S33" s="10" t="str">
         <f t="shared" si="3"/>
@@ -8850,7 +8851,7 @@
         <v>564</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="M40" s="13"/>
       <c r="N40" s="13" t="s">
@@ -9236,7 +9237,7 @@
     </row>
     <row r="46" spans="1:24" ht="30">
       <c r="A46" s="11" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>22</v>
@@ -9266,7 +9267,7 @@
         <v>564</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="M46" s="13"/>
       <c r="N46" s="13" t="s">
@@ -9281,7 +9282,7 @@
         <v>piClim-2xNOx</v>
       </c>
       <c r="R46" s="29" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="S46" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9489,7 +9490,7 @@
         <v>1pctCO2Ndep</v>
       </c>
       <c r="R49" s="8" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="S49" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9934,7 +9935,7 @@
         <v>ssp585-over-bgc</v>
       </c>
       <c r="R55" s="29" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="S55" s="10" t="str">
         <f t="shared" si="3"/>
@@ -10700,7 +10701,7 @@
         <v>amip-piForcing</v>
       </c>
       <c r="R66" s="29" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="S66" s="10" t="s">
         <v>720</v>
@@ -12265,7 +12266,7 @@
         <v>esm-piControl-spinup</v>
       </c>
       <c r="R88" s="8" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="S88" s="10" t="str">
         <f t="shared" si="14"/>
@@ -13005,7 +13006,7 @@
     </row>
     <row r="99" spans="1:24" ht="90">
       <c r="A99" s="11" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>148</v>
@@ -13230,7 +13231,7 @@
     </row>
     <row r="102" spans="1:24" ht="165">
       <c r="A102" s="11" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>156</v>
@@ -13454,7 +13455,7 @@
     </row>
     <row r="105" spans="1:24" ht="60">
       <c r="A105" s="11" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>164</v>
@@ -13602,7 +13603,7 @@
     </row>
     <row r="107" spans="1:24" ht="180">
       <c r="A107" s="11" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>165</v>
@@ -13727,10 +13728,10 @@
         <v>995</v>
       </c>
       <c r="S108" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T108" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U108" s="36" t="str">
         <f t="shared" ref="U108:U140" si="24">IF(T108="", "", "none")</f>
@@ -13740,7 +13741,7 @@
         <v>168</v>
       </c>
       <c r="W108" s="71" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="X108" s="74">
         <f t="shared" si="13"/>
@@ -13792,10 +13793,10 @@
         <v>996</v>
       </c>
       <c r="S109" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T109" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U109" s="36" t="str">
         <f t="shared" si="24"/>
@@ -13859,10 +13860,10 @@
         <v>558</v>
       </c>
       <c r="R110" s="70" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="S110" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T110" s="72"/>
       <c r="U110" s="36" t="str">
@@ -13921,10 +13922,10 @@
         <v>967</v>
       </c>
       <c r="R111" s="8" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="S111" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T111" s="72"/>
       <c r="U111" s="36" t="str">
@@ -13979,7 +13980,7 @@
       </c>
       <c r="S112" s="10"/>
       <c r="T112" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U112" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14037,7 +14038,7 @@
       </c>
       <c r="S113" s="10"/>
       <c r="T113" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U113" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14106,10 +14107,10 @@
         <v>999</v>
       </c>
       <c r="S114" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T114" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U114" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14176,13 +14177,13 @@
         <v>529</v>
       </c>
       <c r="R115" s="8" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="S115" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T115" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U115" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14250,10 +14251,10 @@
         <v>1000</v>
       </c>
       <c r="S116" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T116" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U116" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14312,7 +14313,7 @@
       </c>
       <c r="S117" s="10"/>
       <c r="T117" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U117" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14370,7 +14371,7 @@
       </c>
       <c r="S118" s="10"/>
       <c r="T118" s="73" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="U118" s="36" t="str">
         <f t="shared" si="24"/>
@@ -14439,7 +14440,7 @@
         <v>594</v>
       </c>
       <c r="S119" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T119" s="10"/>
       <c r="U119" s="36" t="str">
@@ -14511,7 +14512,7 @@
         <v>595</v>
       </c>
       <c r="S120" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T120" s="10"/>
       <c r="U120" s="36" t="str">
@@ -14583,7 +14584,7 @@
         <v>596</v>
       </c>
       <c r="S121" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T121" s="10"/>
       <c r="U121" s="36" t="str">
@@ -14653,7 +14654,7 @@
         <v>597</v>
       </c>
       <c r="S122" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T122" s="10"/>
       <c r="U122" s="36" t="str">
@@ -14723,7 +14724,7 @@
         <v>1002</v>
       </c>
       <c r="S123" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T123" s="10"/>
       <c r="U123" s="36" t="str">
@@ -14793,7 +14794,7 @@
         <v>1003</v>
       </c>
       <c r="S124" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T124" s="10"/>
       <c r="U124" s="36" t="str">
@@ -14863,7 +14864,7 @@
         <v>598</v>
       </c>
       <c r="S125" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T125" s="10"/>
       <c r="U125" s="36" t="str">
@@ -14932,10 +14933,10 @@
         <v>539</v>
       </c>
       <c r="R126" s="8" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="S126" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T126" s="10"/>
       <c r="U126" s="36" t="str">
@@ -15007,7 +15008,7 @@
         <v>599</v>
       </c>
       <c r="S127" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T127" s="10"/>
       <c r="U127" s="36" t="str">
@@ -15076,10 +15077,10 @@
         <v>540</v>
       </c>
       <c r="R128" s="8" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="S128" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T128" s="10"/>
       <c r="U128" s="36" t="str">
@@ -15138,10 +15139,10 @@
         <v>970</v>
       </c>
       <c r="R129" s="8" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="S129" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T129" s="10"/>
       <c r="U129" s="36" t="str">
@@ -15200,10 +15201,10 @@
         <v>970</v>
       </c>
       <c r="R130" s="8" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="S130" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T130" s="10"/>
       <c r="U130" s="36" t="str">
@@ -15267,7 +15268,7 @@
         <v>1004</v>
       </c>
       <c r="S131" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T131" s="10"/>
       <c r="U131" s="36" t="str">
@@ -15331,7 +15332,7 @@
         <v>1005</v>
       </c>
       <c r="S132" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T132" s="10"/>
       <c r="U132" s="36" t="str">
@@ -15395,7 +15396,7 @@
         <v>1006</v>
       </c>
       <c r="S133" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T133" s="10"/>
       <c r="U133" s="36" t="str">
@@ -15516,10 +15517,10 @@
         <v>556</v>
       </c>
       <c r="S135" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T135" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U135" s="36" t="str">
         <f t="shared" si="24"/>
@@ -15586,10 +15587,10 @@
         <v>548</v>
       </c>
       <c r="S136" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T136" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U136" s="36" t="str">
         <f t="shared" si="24"/>
@@ -15656,10 +15657,10 @@
         <v>549</v>
       </c>
       <c r="S137" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T137" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U137" s="36" t="str">
         <f t="shared" si="24"/>
@@ -15729,10 +15730,10 @@
         <v>553</v>
       </c>
       <c r="S138" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T138" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U138" s="36" t="str">
         <f t="shared" si="24"/>
@@ -15802,10 +15803,10 @@
         <v>554</v>
       </c>
       <c r="S139" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T139" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U139" s="36" t="str">
         <f t="shared" si="24"/>
@@ -15875,10 +15876,10 @@
         <v>555</v>
       </c>
       <c r="S140" s="10" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T140" s="73" t="s">
-        <v>1014</v>
+        <v>1072</v>
       </c>
       <c r="U140" s="36" t="str">
         <f t="shared" si="24"/>
@@ -16373,7 +16374,7 @@
         <v>piSST-4xCO2-solar</v>
       </c>
       <c r="R147" s="8" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="S147" s="10" t="str">
         <f t="shared" si="26"/>
@@ -16447,7 +16448,7 @@
         <v>futureSST-4xCO2-solar</v>
       </c>
       <c r="R148" s="8" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="S148" s="10" t="str">
         <f t="shared" si="26"/>
@@ -16884,7 +16885,7 @@
         <v>G7cirrus</v>
       </c>
       <c r="R154" s="8" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="S154" s="10" t="str">
         <f t="shared" si="26"/>
@@ -16956,7 +16957,7 @@
         <v>G7SST1-cirrus</v>
       </c>
       <c r="R155" s="8" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="S155" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17104,7 +17105,7 @@
         <v>amip-hist</v>
       </c>
       <c r="R157" s="29" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="S157" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17120,7 +17121,7 @@
         <v/>
       </c>
       <c r="W157" s="23" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="X157" s="74">
         <f t="shared" si="27"/>
@@ -17129,7 +17130,7 @@
     </row>
     <row r="158" spans="1:24" ht="45">
       <c r="A158" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B158" s="14" t="s">
         <v>230</v>
@@ -17180,7 +17181,7 @@
         <v>amip-hld</v>
       </c>
       <c r="R158" s="29" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="S158" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17254,7 +17255,7 @@
         <v>amip-TIP</v>
       </c>
       <c r="R159" s="29" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="S159" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17277,7 +17278,7 @@
     </row>
     <row r="160" spans="1:24" ht="45">
       <c r="A160" s="11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B160" s="14" t="s">
         <v>235</v>
@@ -17330,7 +17331,7 @@
         <v>amip-TIP-nosh</v>
       </c>
       <c r="R160" s="29" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="S160" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17353,7 +17354,7 @@
     </row>
     <row r="161" spans="1:24" ht="60">
       <c r="A161" s="11" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B161" s="14" t="s">
         <v>237</v>
@@ -17404,7 +17405,7 @@
         <v>hist-resAMO</v>
       </c>
       <c r="R161" s="29" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="S161" s="10" t="str">
         <f t="shared" si="26"/>
@@ -17429,7 +17430,7 @@
     </row>
     <row r="162" spans="1:24" ht="75">
       <c r="A162" s="11" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B162" s="14" t="s">
         <v>239</v>
@@ -17480,7 +17481,7 @@
         <v>hist-resIPO</v>
       </c>
       <c r="R162" s="29" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="S162" s="10" t="str">
         <f t="shared" si="26"/>
@@ -19175,7 +19176,7 @@
         <v/>
       </c>
       <c r="W185" s="78" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="X185" s="74">
         <f t="shared" si="27"/>
@@ -20481,7 +20482,7 @@
         <v/>
       </c>
       <c r="W203" s="68" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="X203" s="74"/>
     </row>
@@ -21426,7 +21427,7 @@
         <v>omip1</v>
       </c>
       <c r="K217" s="13" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="L217" s="13"/>
       <c r="M217" s="13"/>
@@ -21442,7 +21443,7 @@
         <v>omip1</v>
       </c>
       <c r="R217" s="8" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="S217" s="10" t="str">
         <f t="shared" si="43"/>
@@ -21465,7 +21466,7 @@
     </row>
     <row r="218" spans="1:24" ht="75">
       <c r="A218" s="76" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B218" s="14" t="s">
         <v>806</v>
@@ -21496,7 +21497,7 @@
         <v>omip1-spunup</v>
       </c>
       <c r="K218" s="13" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="L218" s="13" t="s">
         <v>562</v>
@@ -21513,7 +21514,7 @@
         <v>omip1-spunup</v>
       </c>
       <c r="R218" s="8" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="S218" s="10" t="str">
         <f t="shared" si="43"/>
@@ -21567,7 +21568,7 @@
         <v>omip2</v>
       </c>
       <c r="K219" s="20" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="L219" s="13"/>
       <c r="M219" s="13"/>
@@ -21606,7 +21607,7 @@
     </row>
     <row r="220" spans="1:24" ht="75">
       <c r="A220" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B220" s="14" t="s">
         <v>806</v>
@@ -21637,7 +21638,7 @@
         <v>omip2-spunup</v>
       </c>
       <c r="K220" s="20" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="L220" s="20" t="s">
         <v>562</v>
@@ -23212,7 +23213,7 @@
         <v>hist-spAerO3</v>
       </c>
       <c r="R242" s="29" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="S242" s="10" t="str">
         <f t="shared" si="43"/>
@@ -23288,7 +23289,7 @@
         <v>hist-all-spAerO3</v>
       </c>
       <c r="R243" s="29" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="S243" s="10" t="str">
         <f t="shared" si="43"/>
@@ -23444,7 +23445,7 @@
         <v>505</v>
       </c>
       <c r="R246" s="29" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="S246" s="10" t="str">
         <f t="shared" si="43"/>
@@ -24689,7 +24690,7 @@
         <v>349</v>
       </c>
       <c r="N264" s="15" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="O264" s="14" t="s">
         <v>17</v>
@@ -24705,7 +24706,7 @@
         <v>909</v>
       </c>
       <c r="S264" s="31" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="T264" s="10"/>
       <c r="U264" s="36" t="str">
@@ -25015,7 +25016,7 @@
     </row>
     <row r="269" spans="1:24" ht="60">
       <c r="A269" s="11" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B269" s="14"/>
       <c r="C269" s="26" t="s">
@@ -25050,7 +25051,7 @@
         <v>899</v>
       </c>
       <c r="M269" s="13" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="N269" s="13" t="s">
         <v>720</v>
@@ -25066,7 +25067,7 @@
         <v>volc-cluster-21C</v>
       </c>
       <c r="R269" s="8" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S269" s="10" t="str">
         <f t="shared" si="43"/>
@@ -25122,7 +25123,7 @@
         <v>902</v>
       </c>
       <c r="M270" s="13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="N270" s="13" t="s">
         <v>720</v>
@@ -25138,7 +25139,7 @@
         <v>volc-long-hlS</v>
       </c>
       <c r="R270" s="8" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="S270" s="10" t="str">
         <f t="shared" si="43"/>
@@ -25163,11 +25164,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
     <mergeCell ref="B1:R1"/>
     <mergeCell ref="B10:R10"/>
     <mergeCell ref="K11:M11"/>
@@ -25176,6 +25172,11 @@
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>